<commit_message>
📊 Weekly driver report update for 2025-04-20
</commit_message>
<xml_diff>
--- a/Output/roaming_impact_reports_per_acct/ABM_driver_summary.xlsx
+++ b/Output/roaming_impact_reports_per_acct/ABM_driver_summary.xlsx
@@ -557,8 +557,10 @@
       <c r="D12" s="4" t="n">
         <v>100</v>
       </c>
-      <c r="E12" s="4" t="n">
-        <v/>
+      <c r="E12" s="4" t="inlineStr">
+        <is>
+          <t>2022-08-29</t>
+        </is>
       </c>
     </row>
     <row r="13">

</xml_diff>

<commit_message>
📊 Weekly driver report update for 2025-04-21
</commit_message>
<xml_diff>
--- a/Output/roaming_impact_reports_per_acct/ABM_driver_summary.xlsx
+++ b/Output/roaming_impact_reports_per_acct/ABM_driver_summary.xlsx
@@ -490,7 +490,7 @@
         <v>1</v>
       </c>
       <c r="C3" s="4" t="n">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D3" s="4" t="n">
         <v>98.7</v>
@@ -506,7 +506,7 @@
         <v>1</v>
       </c>
       <c r="C4" s="5" t="n">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="5"/>

</xml_diff>

<commit_message>
📊 Weekly driver report update for 2025-04-28
</commit_message>
<xml_diff>
--- a/Output/roaming_impact_reports_per_acct/ABM_driver_summary.xlsx
+++ b/Output/roaming_impact_reports_per_acct/ABM_driver_summary.xlsx
@@ -551,7 +551,7 @@
         </is>
       </c>
       <c r="B12" s="6" t="n">
-        <v>10661</v>
+        <v>11140</v>
       </c>
       <c r="C12" t="inlineStr"/>
       <c r="D12" s="4" t="n">
@@ -570,7 +570,7 @@
         </is>
       </c>
       <c r="B13" s="6" t="n">
-        <v>14239</v>
+        <v>14487</v>
       </c>
       <c r="C13" t="inlineStr"/>
       <c r="D13" s="4" t="n">

</xml_diff>

<commit_message>
📊 Weekly driver report update for 2025-04-29
</commit_message>
<xml_diff>
--- a/Output/roaming_impact_reports_per_acct/ABM_driver_summary.xlsx
+++ b/Output/roaming_impact_reports_per_acct/ABM_driver_summary.xlsx
@@ -52,7 +52,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
@@ -63,9 +63,6 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="3" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="right"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -431,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J19"/>
+  <dimension ref="A1:J24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -440,15 +437,15 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col width="45" customWidth="1" min="1" max="1"/>
-    <col width="15" customWidth="1" min="2" max="2"/>
+    <col width="14" customWidth="1" min="2" max="2"/>
     <col width="18" customWidth="1" min="3" max="3"/>
     <col width="30" customWidth="1" min="4" max="4"/>
-    <col width="16" customWidth="1" min="5" max="5"/>
-    <col width="2" customWidth="1" min="6" max="6"/>
-    <col width="2" customWidth="1" min="7" max="7"/>
-    <col width="2" customWidth="1" min="8" max="8"/>
-    <col width="2" customWidth="1" min="9" max="9"/>
-    <col width="2" customWidth="1" min="10" max="10"/>
+    <col width="14" customWidth="1" min="5" max="5"/>
+    <col width="11" customWidth="1" min="6" max="6"/>
+    <col width="32" customWidth="1" min="7" max="7"/>
+    <col width="12" customWidth="1" min="8" max="8"/>
+    <col width="30" customWidth="1" min="9" max="9"/>
+    <col width="16" customWidth="1" min="10" max="10"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -522,90 +519,577 @@
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="2" t="inlineStr">
-        <is>
-          <t>Adapter-Driver</t>
-        </is>
-      </c>
-      <c r="B11" s="3" t="inlineStr">
-        <is>
-          <t>Total Samples</t>
-        </is>
-      </c>
-      <c r="C11" s="2" t="inlineStr"/>
-      <c r="D11" s="3" t="inlineStr">
-        <is>
-          <t>Good Roaming Calculation (%)</t>
-        </is>
-      </c>
-      <c r="E11" s="3" t="inlineStr">
-        <is>
-          <t>Driver Vintage</t>
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>adapter-driver</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>good sum</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>critical sum</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>warning sum</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>client count</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>total sum</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>adapter</t>
+        </is>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>driver</t>
+        </is>
+      </c>
+      <c r="I11" t="inlineStr">
+        <is>
+          <t>good roaming calculation (%)</t>
+        </is>
+      </c>
+      <c r="J11" t="inlineStr">
+        <is>
+          <t>driver vintage</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Intel(R) Wi-Fi 6E AX211 160MHz - 22.150.3.1</t>
-        </is>
-      </c>
-      <c r="B12" s="6" t="n">
-        <v>11140</v>
-      </c>
-      <c r="C12" t="inlineStr"/>
-      <c r="D12" s="4" t="n">
-        <v>100</v>
-      </c>
-      <c r="E12" s="4" t="inlineStr">
-        <is>
-          <t>2022-08-29</t>
+          <t>Intel(R) Wi-Fi 6E AX211 160MHz - 22.180.0.4</t>
+        </is>
+      </c>
+      <c r="B12" t="n">
+        <v>17609</v>
+      </c>
+      <c r="C12" t="n">
+        <v>69</v>
+      </c>
+      <c r="D12" t="n">
+        <v>0</v>
+      </c>
+      <c r="E12" t="n">
+        <v>57</v>
+      </c>
+      <c r="F12" t="n">
+        <v>17678</v>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>intel(r) wi-fi 6e ax211 160mhz</t>
+        </is>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>22.180.0.4</t>
+        </is>
+      </c>
+      <c r="I12" t="n">
+        <v>99.59999999999999</v>
+      </c>
+      <c r="J12" t="inlineStr">
+        <is>
+          <t>2022-10-17</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Intel(R) Wi-Fi 6E AX211 160MHz - 22.150.0.3</t>
-        </is>
-      </c>
-      <c r="B13" s="6" t="n">
-        <v>14487</v>
-      </c>
-      <c r="C13" t="inlineStr"/>
-      <c r="D13" s="4" t="n">
-        <v>100</v>
-      </c>
-      <c r="E13" s="4" t="inlineStr">
-        <is>
-          <t>2022-05-23</t>
+          <t>Intel(R) Wi-Fi 6E AX211 160MHz - 22.250.0.4</t>
+        </is>
+      </c>
+      <c r="B13" t="n">
+        <v>1254472</v>
+      </c>
+      <c r="C13" t="n">
+        <v>4270</v>
+      </c>
+      <c r="D13" t="n">
+        <v>1009</v>
+      </c>
+      <c r="E13" t="n">
+        <v>1946</v>
+      </c>
+      <c r="F13" t="n">
+        <v>1259751</v>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>intel(r) wi-fi 6e ax211 160mhz</t>
+        </is>
+      </c>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>22.250.0.4</t>
+        </is>
+      </c>
+      <c r="I13" t="n">
+        <v>99.59999999999999</v>
+      </c>
+      <c r="J13" t="inlineStr">
+        <is>
+          <t>2023-07-25</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
+          <t>Intel(R) Wi-Fi 6E AX211 160MHz - 23.10.0.8</t>
+        </is>
+      </c>
+      <c r="B14" t="n">
+        <v>448248</v>
+      </c>
+      <c r="C14" t="n">
+        <v>738</v>
+      </c>
+      <c r="D14" t="n">
+        <v>931</v>
+      </c>
+      <c r="E14" t="n">
+        <v>688</v>
+      </c>
+      <c r="F14" t="n">
+        <v>449917</v>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>intel(r) wi-fi 6e ax211 160mhz</t>
+        </is>
+      </c>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t>23.10.0.8</t>
+        </is>
+      </c>
+      <c r="I14" t="n">
+        <v>99.59999999999999</v>
+      </c>
+      <c r="J14" t="inlineStr">
+        <is>
+          <t>2023-10-30</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>Intel(R) Wi-Fi 6E AX211 160MHz - 23.120.0.3</t>
+        </is>
+      </c>
+      <c r="B15" t="n">
+        <v>204134</v>
+      </c>
+      <c r="C15" t="n">
+        <v>775</v>
+      </c>
+      <c r="D15" t="n">
+        <v>52</v>
+      </c>
+      <c r="E15" t="n">
+        <v>319</v>
+      </c>
+      <c r="F15" t="n">
+        <v>204961</v>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>intel(r) wi-fi 6e ax211 160mhz</t>
+        </is>
+      </c>
+      <c r="H15" t="inlineStr">
+        <is>
+          <t>23.120.0.3</t>
+        </is>
+      </c>
+      <c r="I15" t="n">
+        <v>99.59999999999999</v>
+      </c>
+      <c r="J15" t="inlineStr">
+        <is>
+          <t>2025-02-05</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>Intel(R) Wi-Fi 6E AX211 160MHz - 22.220.0.4</t>
+        </is>
+      </c>
+      <c r="B16" t="n">
+        <v>28296</v>
+      </c>
+      <c r="C16" t="n">
+        <v>111</v>
+      </c>
+      <c r="D16" t="n">
+        <v>0</v>
+      </c>
+      <c r="E16" t="n">
+        <v>61</v>
+      </c>
+      <c r="F16" t="n">
+        <v>28407</v>
+      </c>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>intel(r) wi-fi 6e ax211 160mhz</t>
+        </is>
+      </c>
+      <c r="H16" t="inlineStr">
+        <is>
+          <t>22.220.0.4</t>
+        </is>
+      </c>
+      <c r="I16" t="n">
+        <v>99.59999999999999</v>
+      </c>
+      <c r="J16" t="inlineStr">
+        <is>
+          <t>2023-03-28</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>Intel(R) Wi-Fi 6E AX211 160MHz - 22.230.0.8</t>
+        </is>
+      </c>
+      <c r="B17" t="n">
+        <v>1734330</v>
+      </c>
+      <c r="C17" t="n">
+        <v>2979</v>
+      </c>
+      <c r="D17" t="n">
+        <v>2614</v>
+      </c>
+      <c r="E17" t="n">
+        <v>2960</v>
+      </c>
+      <c r="F17" t="n">
+        <v>1739923</v>
+      </c>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>intel(r) wi-fi 6e ax211 160mhz</t>
+        </is>
+      </c>
+      <c r="H17" t="inlineStr">
+        <is>
+          <t>22.230.0.8</t>
+        </is>
+      </c>
+      <c r="I17" t="n">
+        <v>99.7</v>
+      </c>
+      <c r="J17" t="inlineStr">
+        <is>
+          <t>2023-05-08</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>Intel(R) Wi-Fi 6E AX211 160MHz - 22.110.1.1</t>
+        </is>
+      </c>
+      <c r="B18" t="n">
+        <v>134169</v>
+      </c>
+      <c r="C18" t="n">
+        <v>189</v>
+      </c>
+      <c r="D18" t="n">
+        <v>263</v>
+      </c>
+      <c r="E18" t="n">
+        <v>192</v>
+      </c>
+      <c r="F18" t="n">
+        <v>134621</v>
+      </c>
+      <c r="G18" t="inlineStr">
+        <is>
+          <t>intel(r) wi-fi 6e ax211 160mhz</t>
+        </is>
+      </c>
+      <c r="H18" t="inlineStr">
+        <is>
+          <t>22.110.1.1</t>
+        </is>
+      </c>
+      <c r="I18" t="n">
+        <v>99.7</v>
+      </c>
+      <c r="J18" t="inlineStr">
+        <is>
+          <t>2022-01-01</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>Intel(R) Wi-Fi 6E AX211 160MHz - 23.70.2.3</t>
+        </is>
+      </c>
+      <c r="B19" t="n">
+        <v>210370</v>
+      </c>
+      <c r="C19" t="n">
+        <v>324</v>
+      </c>
+      <c r="D19" t="n">
+        <v>313</v>
+      </c>
+      <c r="E19" t="n">
+        <v>558</v>
+      </c>
+      <c r="F19" t="n">
+        <v>211007</v>
+      </c>
+      <c r="G19" t="inlineStr">
+        <is>
+          <t>intel(r) wi-fi 6e ax211 160mhz</t>
+        </is>
+      </c>
+      <c r="H19" t="inlineStr">
+        <is>
+          <t>23.70.2.3</t>
+        </is>
+      </c>
+      <c r="I19" t="n">
+        <v>99.7</v>
+      </c>
+      <c r="J19" t="inlineStr">
+        <is>
+          <t>2024-07-23</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>Intel(R) Wi-Fi 6E AX211 160MHz - 23.80.1.3</t>
+        </is>
+      </c>
+      <c r="B20" t="n">
+        <v>140350</v>
+      </c>
+      <c r="C20" t="n">
+        <v>270</v>
+      </c>
+      <c r="D20" t="n">
+        <v>75</v>
+      </c>
+      <c r="E20" t="n">
+        <v>307</v>
+      </c>
+      <c r="F20" t="n">
+        <v>140695</v>
+      </c>
+      <c r="G20" t="inlineStr">
+        <is>
+          <t>intel(r) wi-fi 6e ax211 160mhz</t>
+        </is>
+      </c>
+      <c r="H20" t="inlineStr">
+        <is>
+          <t>23.80.1.3</t>
+        </is>
+      </c>
+      <c r="I20" t="n">
+        <v>99.8</v>
+      </c>
+      <c r="J20" t="inlineStr">
+        <is>
+          <t>2024-09-03</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>Intel(R) Wi-Fi 6E AX211 160MHz - 23.100.0.4</t>
+        </is>
+      </c>
+      <c r="B21" t="n">
+        <v>230530</v>
+      </c>
+      <c r="C21" t="n">
+        <v>421</v>
+      </c>
+      <c r="D21" t="n">
+        <v>37</v>
+      </c>
+      <c r="E21" t="n">
+        <v>399</v>
+      </c>
+      <c r="F21" t="n">
+        <v>230988</v>
+      </c>
+      <c r="G21" t="inlineStr">
+        <is>
+          <t>intel(r) wi-fi 6e ax211 160mhz</t>
+        </is>
+      </c>
+      <c r="H21" t="inlineStr">
+        <is>
+          <t>23.100.0.4</t>
+        </is>
+      </c>
+      <c r="I21" t="n">
+        <v>99.8</v>
+      </c>
+      <c r="J21" t="inlineStr">
+        <is>
+          <t>2024-11-10</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
           <t>Intel(R) Wi-Fi 6E AX211 160MHz - 22.100.1.1</t>
         </is>
       </c>
-      <c r="B14" s="6" t="n">
+      <c r="B22" t="n">
+        <v>265066</v>
+      </c>
+      <c r="C22" t="n">
+        <v>203</v>
+      </c>
+      <c r="D22" t="n">
+        <v>131</v>
+      </c>
+      <c r="E22" t="n">
+        <v>310</v>
+      </c>
+      <c r="F22" t="n">
         <v>265400</v>
       </c>
-      <c r="C14" t="inlineStr"/>
-      <c r="D14" s="4" t="n">
+      <c r="G22" t="inlineStr">
+        <is>
+          <t>intel(r) wi-fi 6e ax211 160mhz</t>
+        </is>
+      </c>
+      <c r="H22" t="inlineStr">
+        <is>
+          <t>22.100.1.1</t>
+        </is>
+      </c>
+      <c r="I22" t="n">
         <v>99.90000000000001</v>
       </c>
-      <c r="E14" s="4" t="inlineStr">
+      <c r="J22" t="inlineStr">
         <is>
           <t>2022-05-01</t>
         </is>
       </c>
     </row>
-    <row r="15"/>
-    <row r="16"/>
-    <row r="17"/>
-    <row r="18"/>
-    <row r="19"/>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>Intel(R) Wi-Fi 6E AX211 160MHz - 22.150.0.3</t>
+        </is>
+      </c>
+      <c r="B23" t="n">
+        <v>14487</v>
+      </c>
+      <c r="C23" t="n">
+        <v>0</v>
+      </c>
+      <c r="D23" t="n">
+        <v>0</v>
+      </c>
+      <c r="E23" t="n">
+        <v>57</v>
+      </c>
+      <c r="F23" t="n">
+        <v>14487</v>
+      </c>
+      <c r="G23" t="inlineStr">
+        <is>
+          <t>intel(r) wi-fi 6e ax211 160mhz</t>
+        </is>
+      </c>
+      <c r="H23" t="inlineStr">
+        <is>
+          <t>22.150.0.3</t>
+        </is>
+      </c>
+      <c r="I23" t="n">
+        <v>100</v>
+      </c>
+      <c r="J23" t="inlineStr">
+        <is>
+          <t>2022-05-23</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>Intel(R) Wi-Fi 6E AX211 160MHz - 22.150.3.1</t>
+        </is>
+      </c>
+      <c r="B24" t="n">
+        <v>11140</v>
+      </c>
+      <c r="C24" t="n">
+        <v>0</v>
+      </c>
+      <c r="D24" t="n">
+        <v>0</v>
+      </c>
+      <c r="E24" t="n">
+        <v>59</v>
+      </c>
+      <c r="F24" t="n">
+        <v>11140</v>
+      </c>
+      <c r="G24" t="inlineStr">
+        <is>
+          <t>intel(r) wi-fi 6e ax211 160mhz</t>
+        </is>
+      </c>
+      <c r="H24" t="inlineStr">
+        <is>
+          <t>22.150.3.1</t>
+        </is>
+      </c>
+      <c r="I24" t="n">
+        <v>100</v>
+      </c>
+      <c r="J24" t="inlineStr">
+        <is>
+          <t>2022-08-29</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
📊 Weekly driver report update for 2025-05-05
</commit_message>
<xml_diff>
--- a/Output/roaming_impact_reports_per_acct/ABM_driver_summary.xlsx
+++ b/Output/roaming_impact_reports_per_acct/ABM_driver_summary.xlsx
@@ -484,13 +484,13 @@
         </is>
       </c>
       <c r="B3" s="4" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C3" s="4" t="n">
-        <v>125</v>
+        <v>218</v>
       </c>
       <c r="D3" s="4" t="n">
-        <v>98.7</v>
+        <v>98.59999999999999</v>
       </c>
     </row>
     <row r="4">
@@ -500,10 +500,10 @@
         </is>
       </c>
       <c r="B4" s="5" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C4" s="5" t="n">
-        <v>125</v>
+        <v>218</v>
       </c>
     </row>
     <row r="5"/>
@@ -617,19 +617,19 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>1254472</v>
+        <v>1293197</v>
       </c>
       <c r="C13" t="n">
-        <v>4270</v>
+        <v>4322</v>
       </c>
       <c r="D13" t="n">
         <v>1009</v>
       </c>
       <c r="E13" t="n">
-        <v>1946</v>
+        <v>1990</v>
       </c>
       <c r="F13" t="n">
-        <v>1259751</v>
+        <v>1298528</v>
       </c>
       <c r="G13" t="inlineStr">
         <is>
@@ -653,23 +653,23 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Intel(R) Wi-Fi 6E AX211 160MHz - 23.10.0.8</t>
+          <t>Intel(R) Wi-Fi 6E AX211 160MHz - 22.220.0.4</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>448248</v>
+        <v>31517</v>
       </c>
       <c r="C14" t="n">
-        <v>738</v>
+        <v>112</v>
       </c>
       <c r="D14" t="n">
-        <v>931</v>
+        <v>0</v>
       </c>
       <c r="E14" t="n">
-        <v>688</v>
+        <v>66</v>
       </c>
       <c r="F14" t="n">
-        <v>449917</v>
+        <v>31629</v>
       </c>
       <c r="G14" t="inlineStr">
         <is>
@@ -678,7 +678,7 @@
       </c>
       <c r="H14" t="inlineStr">
         <is>
-          <t>23.10.0.8</t>
+          <t>22.220.0.4</t>
         </is>
       </c>
       <c r="I14" t="n">
@@ -686,30 +686,30 @@
       </c>
       <c r="J14" t="inlineStr">
         <is>
-          <t>2023-10-30</t>
+          <t>2023-03-28</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Intel(R) Wi-Fi 6E AX211 160MHz - 23.120.0.3</t>
+          <t>Intel(R) Wi-Fi 6E AX211 160MHz - 23.10.0.8</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>204134</v>
+        <v>467311</v>
       </c>
       <c r="C15" t="n">
-        <v>775</v>
+        <v>772</v>
       </c>
       <c r="D15" t="n">
-        <v>52</v>
+        <v>931</v>
       </c>
       <c r="E15" t="n">
-        <v>319</v>
+        <v>706</v>
       </c>
       <c r="F15" t="n">
-        <v>204961</v>
+        <v>469014</v>
       </c>
       <c r="G15" t="inlineStr">
         <is>
@@ -718,7 +718,7 @@
       </c>
       <c r="H15" t="inlineStr">
         <is>
-          <t>23.120.0.3</t>
+          <t>23.10.0.8</t>
         </is>
       </c>
       <c r="I15" t="n">
@@ -726,30 +726,30 @@
       </c>
       <c r="J15" t="inlineStr">
         <is>
-          <t>2025-02-05</t>
+          <t>2023-10-30</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Intel(R) Wi-Fi 6E AX211 160MHz - 22.220.0.4</t>
+          <t>Intel(R) Wi-Fi 6E AX211 160MHz - 23.120.0.3</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>28296</v>
+        <v>455081</v>
       </c>
       <c r="C16" t="n">
-        <v>111</v>
+        <v>1861</v>
       </c>
       <c r="D16" t="n">
-        <v>0</v>
+        <v>52</v>
       </c>
       <c r="E16" t="n">
-        <v>61</v>
+        <v>639</v>
       </c>
       <c r="F16" t="n">
-        <v>28407</v>
+        <v>456994</v>
       </c>
       <c r="G16" t="inlineStr">
         <is>
@@ -758,7 +758,7 @@
       </c>
       <c r="H16" t="inlineStr">
         <is>
-          <t>22.220.0.4</t>
+          <t>23.120.0.3</t>
         </is>
       </c>
       <c r="I16" t="n">
@@ -766,7 +766,7 @@
       </c>
       <c r="J16" t="inlineStr">
         <is>
-          <t>2023-03-28</t>
+          <t>2025-02-05</t>
         </is>
       </c>
     </row>
@@ -777,19 +777,19 @@
         </is>
       </c>
       <c r="B17" t="n">
-        <v>1734330</v>
+        <v>1787924</v>
       </c>
       <c r="C17" t="n">
-        <v>2979</v>
+        <v>3326</v>
       </c>
       <c r="D17" t="n">
         <v>2614</v>
       </c>
       <c r="E17" t="n">
-        <v>2960</v>
+        <v>3038</v>
       </c>
       <c r="F17" t="n">
-        <v>1739923</v>
+        <v>1793864</v>
       </c>
       <c r="G17" t="inlineStr">
         <is>
@@ -813,23 +813,23 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Intel(R) Wi-Fi 6E AX211 160MHz - 22.110.1.1</t>
+          <t>Intel(R) Wi-Fi 6E AX211 160MHz - 23.70.2.3</t>
         </is>
       </c>
       <c r="B18" t="n">
-        <v>134169</v>
+        <v>218767</v>
       </c>
       <c r="C18" t="n">
-        <v>189</v>
+        <v>334</v>
       </c>
       <c r="D18" t="n">
-        <v>263</v>
+        <v>313</v>
       </c>
       <c r="E18" t="n">
-        <v>192</v>
+        <v>573</v>
       </c>
       <c r="F18" t="n">
-        <v>134621</v>
+        <v>219414</v>
       </c>
       <c r="G18" t="inlineStr">
         <is>
@@ -838,7 +838,7 @@
       </c>
       <c r="H18" t="inlineStr">
         <is>
-          <t>22.110.1.1</t>
+          <t>23.70.2.3</t>
         </is>
       </c>
       <c r="I18" t="n">
@@ -846,30 +846,30 @@
       </c>
       <c r="J18" t="inlineStr">
         <is>
-          <t>2022-01-01</t>
+          <t>2024-07-23</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>Intel(R) Wi-Fi 6E AX211 160MHz - 23.70.2.3</t>
+          <t>Intel(R) Wi-Fi 6E AX211 160MHz - 22.110.1.1</t>
         </is>
       </c>
       <c r="B19" t="n">
-        <v>210370</v>
+        <v>135467</v>
       </c>
       <c r="C19" t="n">
-        <v>324</v>
+        <v>189</v>
       </c>
       <c r="D19" t="n">
-        <v>313</v>
+        <v>263</v>
       </c>
       <c r="E19" t="n">
-        <v>558</v>
+        <v>196</v>
       </c>
       <c r="F19" t="n">
-        <v>211007</v>
+        <v>135919</v>
       </c>
       <c r="G19" t="inlineStr">
         <is>
@@ -878,7 +878,7 @@
       </c>
       <c r="H19" t="inlineStr">
         <is>
-          <t>23.70.2.3</t>
+          <t>22.110.1.1</t>
         </is>
       </c>
       <c r="I19" t="n">
@@ -886,30 +886,30 @@
       </c>
       <c r="J19" t="inlineStr">
         <is>
-          <t>2024-07-23</t>
+          <t>2022-01-01</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>Intel(R) Wi-Fi 6E AX211 160MHz - 23.80.1.3</t>
+          <t>Intel(R) Wi-Fi 6E AX211 160MHz - 23.100.0.4</t>
         </is>
       </c>
       <c r="B20" t="n">
-        <v>140350</v>
+        <v>240434</v>
       </c>
       <c r="C20" t="n">
-        <v>270</v>
+        <v>421</v>
       </c>
       <c r="D20" t="n">
-        <v>75</v>
+        <v>37</v>
       </c>
       <c r="E20" t="n">
-        <v>307</v>
+        <v>409</v>
       </c>
       <c r="F20" t="n">
-        <v>140695</v>
+        <v>240892</v>
       </c>
       <c r="G20" t="inlineStr">
         <is>
@@ -918,7 +918,7 @@
       </c>
       <c r="H20" t="inlineStr">
         <is>
-          <t>23.80.1.3</t>
+          <t>23.100.0.4</t>
         </is>
       </c>
       <c r="I20" t="n">
@@ -926,30 +926,30 @@
       </c>
       <c r="J20" t="inlineStr">
         <is>
-          <t>2024-09-03</t>
+          <t>2024-11-10</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>Intel(R) Wi-Fi 6E AX211 160MHz - 23.100.0.4</t>
+          <t>Intel(R) Wi-Fi 6E AX211 160MHz - 23.80.1.3</t>
         </is>
       </c>
       <c r="B21" t="n">
-        <v>230530</v>
+        <v>151287</v>
       </c>
       <c r="C21" t="n">
-        <v>421</v>
+        <v>285</v>
       </c>
       <c r="D21" t="n">
-        <v>37</v>
+        <v>75</v>
       </c>
       <c r="E21" t="n">
-        <v>399</v>
+        <v>332</v>
       </c>
       <c r="F21" t="n">
-        <v>230988</v>
+        <v>151647</v>
       </c>
       <c r="G21" t="inlineStr">
         <is>
@@ -958,7 +958,7 @@
       </c>
       <c r="H21" t="inlineStr">
         <is>
-          <t>23.100.0.4</t>
+          <t>23.80.1.3</t>
         </is>
       </c>
       <c r="I21" t="n">
@@ -966,7 +966,7 @@
       </c>
       <c r="J21" t="inlineStr">
         <is>
-          <t>2024-11-10</t>
+          <t>2024-09-03</t>
         </is>
       </c>
     </row>
@@ -977,19 +977,19 @@
         </is>
       </c>
       <c r="B22" t="n">
-        <v>265066</v>
+        <v>272039</v>
       </c>
       <c r="C22" t="n">
-        <v>203</v>
+        <v>213</v>
       </c>
       <c r="D22" t="n">
         <v>131</v>
       </c>
       <c r="E22" t="n">
-        <v>310</v>
+        <v>316</v>
       </c>
       <c r="F22" t="n">
-        <v>265400</v>
+        <v>272383</v>
       </c>
       <c r="G22" t="inlineStr">
         <is>
@@ -1017,7 +1017,7 @@
         </is>
       </c>
       <c r="B23" t="n">
-        <v>14487</v>
+        <v>14561</v>
       </c>
       <c r="C23" t="n">
         <v>0</v>
@@ -1026,10 +1026,10 @@
         <v>0</v>
       </c>
       <c r="E23" t="n">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="F23" t="n">
-        <v>14487</v>
+        <v>14561</v>
       </c>
       <c r="G23" t="inlineStr">
         <is>
@@ -1057,7 +1057,7 @@
         </is>
       </c>
       <c r="B24" t="n">
-        <v>11140</v>
+        <v>12018</v>
       </c>
       <c r="C24" t="n">
         <v>0</v>
@@ -1066,10 +1066,10 @@
         <v>0</v>
       </c>
       <c r="E24" t="n">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="F24" t="n">
-        <v>11140</v>
+        <v>12018</v>
       </c>
       <c r="G24" t="inlineStr">
         <is>

</xml_diff>